<commit_message>
wave 2005/06 reconciliation with official figures
</commit_message>
<xml_diff>
--- a/UNHS_2005/GAPP2/in/Conversionfactors.xlsx
+++ b/UNHS_2005/GAPP2/in/Conversionfactors.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>untcd</t>
-  </si>
-  <si>
     <t>product</t>
   </si>
   <si>
     <t>convfactor</t>
+  </si>
+  <si>
+    <t>h14aq3</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="765" activePane="bottomLeft"/>
       <selection activeCell="C2" sqref="C2"/>
-      <selection pane="bottomLeft" activeCell="B461" sqref="B461"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -428,13 +428,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>